<commit_message>
tambah frost grey dan maroon
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B266A87-4711-401D-9E53-AF6F5C929432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBA6550-282E-4656-9595-A79BA43AAFD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>Timestamp</t>
   </si>
@@ -204,6 +204,45 @@
   <si>
     <t>frost grey</t>
   </si>
+  <si>
+    <t>Gamis Ibu size XL ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Gamis Ibu size L ( 3 pcs )</t>
+  </si>
+  <si>
+    <t>Koko ayah lengan panjang manset size XL ( 1Pcs )</t>
+  </si>
+  <si>
+    <t>Koko ayah lengan panjang manset size XXL ( 2 pcs )</t>
+  </si>
+  <si>
+    <t>Koko kids size S ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Koko Ayah tangan pendek size L ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Gamis Ibu size L ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Gamis Ibu size S ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Koko kids size L ( 1pcs )</t>
+  </si>
+  <si>
+    <t>koko Kids size M ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Khimar Nurani Dewasa size L ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Khimar Nurani Kids size XXL ( 1pcs )</t>
+  </si>
+  <si>
+    <t>Maroon</t>
+  </si>
 </sst>
 </file>
 
@@ -212,12 +251,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -239,6 +285,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -384,61 +436,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -458,6 +510,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E15418"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -48030,21 +48100,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E5F31-2BCE-4B36-AB40-B45240226FD3}">
-  <dimension ref="B4:E57"/>
+  <dimension ref="A4:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5">
+    <row r="4" spans="1:5">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -48052,7 +48122,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="1:5">
       <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
@@ -48060,7 +48130,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="1:5">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -48074,617 +48144,390 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="5" t="s">
-        <v>6</v>
+    <row r="7" spans="1:5">
+      <c r="A7" s="32" t="s">
+        <v>57</v>
       </c>
-      <c r="C7" s="11">
+      <c r="B7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="31">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
-        <v>0</v>
+      <c r="D7" s="31"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="33"/>
+      <c r="B8" s="30" t="s">
+        <v>59</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="5" t="s">
-        <v>7</v>
+      <c r="C8" s="31">
+        <v>3</v>
       </c>
-      <c r="C8" s="11">
+      <c r="D8" s="31"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="33"/>
+      <c r="B9" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="31">
         <v>1</v>
       </c>
-      <c r="D8" s="12">
-        <v>0</v>
+      <c r="D9" s="31"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="33"/>
+      <c r="B10" s="30" t="s">
+        <v>61</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="C10" s="31">
         <v>2</v>
       </c>
-      <c r="D9" s="12">
-        <v>0</v>
+      <c r="D10" s="31"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="33"/>
+      <c r="B11" s="30" t="s">
+        <v>62</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="C11" s="31">
         <v>1</v>
       </c>
-      <c r="D10" s="12">
-        <v>0</v>
+      <c r="D11" s="31"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="32" t="s">
+        <v>70</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="5" t="s">
-        <v>10</v>
+      <c r="B12" s="30" t="s">
+        <v>63</v>
       </c>
-      <c r="C11" s="11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="C12" s="31">
         <v>1</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="5" t="s">
-        <v>11</v>
+      <c r="D12" s="31"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="33"/>
+      <c r="B13" s="30" t="s">
+        <v>64</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C13" s="31">
         <v>1</v>
       </c>
-      <c r="D12" s="12">
-        <v>0</v>
+      <c r="D13" s="31"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="33"/>
+      <c r="B14" s="30" t="s">
+        <v>65</v>
       </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="2:5">
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="11">
-        <v>0</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="C14" s="31">
         <v>1</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="5" t="s">
-        <v>13</v>
+      <c r="D14" s="31"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="33"/>
+      <c r="B15" s="30" t="s">
+        <v>66</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C15" s="31">
         <v>1</v>
       </c>
-      <c r="D14" s="12">
-        <v>0</v>
+      <c r="D15" s="31"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="33"/>
+      <c r="B16" s="30" t="s">
+        <v>67</v>
       </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0</v>
-      </c>
-      <c r="D15" s="12">
-        <v>2</v>
-      </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="11">
+      <c r="C16" s="31">
         <v>1</v>
       </c>
-      <c r="D16" s="12">
-        <v>0</v>
+      <c r="D16" s="31"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="33"/>
+      <c r="B17" s="30" t="s">
+        <v>68</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="11">
+      <c r="C17" s="31">
         <v>1</v>
       </c>
-      <c r="D17" s="12">
-        <v>0</v>
+      <c r="D17" s="31"/>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="33"/>
+      <c r="B18" s="30" t="s">
+        <v>69</v>
       </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="11">
-        <v>0</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="C18" s="31">
         <v>1</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="11">
-        <v>1</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="11">
-        <v>1</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="11">
-        <v>0</v>
-      </c>
-      <c r="D21" s="12">
-        <v>1</v>
-      </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="11">
-        <v>0</v>
-      </c>
-      <c r="D22" s="12">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="11">
-        <v>0</v>
-      </c>
-      <c r="D23" s="12">
-        <v>1</v>
-      </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="11">
-        <v>1</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="11">
-        <v>0</v>
-      </c>
-      <c r="D25" s="12">
-        <v>2</v>
-      </c>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="11">
-        <v>0</v>
-      </c>
-      <c r="D26" s="12">
-        <v>2</v>
-      </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="11">
-        <v>0</v>
-      </c>
-      <c r="D27" s="12">
-        <v>2</v>
-      </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="11">
-        <v>0</v>
-      </c>
-      <c r="D28" s="12">
-        <v>2</v>
-      </c>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="11">
-        <v>0</v>
-      </c>
-      <c r="D29" s="12">
-        <v>2</v>
-      </c>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="11">
-        <v>0</v>
-      </c>
-      <c r="D30" s="12">
-        <v>1</v>
-      </c>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="11">
-        <v>0</v>
-      </c>
-      <c r="D31" s="12">
-        <v>1</v>
-      </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="11">
-        <v>0</v>
-      </c>
-      <c r="D32" s="12">
-        <v>1</v>
-      </c>
-      <c r="E32" s="10"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="28"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="29"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="29"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="28"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="29"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="29"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="29"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="28"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="29"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="28"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="29"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="28"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="29"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="28"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="29"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="28"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="29"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="28"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="29"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="29"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="28"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="29"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="28"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="11">
-        <v>0</v>
-      </c>
-      <c r="D33" s="12">
-        <v>2</v>
-      </c>
-      <c r="E33" s="10"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="28"/>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="11">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12">
-        <v>1</v>
-      </c>
-      <c r="E34" s="10"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="28"/>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="11">
-        <v>0</v>
-      </c>
-      <c r="D35" s="12">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="28"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="11">
-        <v>3</v>
-      </c>
-      <c r="D36" s="12">
-        <v>0</v>
-      </c>
-      <c r="E36" s="10"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="11">
-        <v>1</v>
-      </c>
-      <c r="D37" s="12">
-        <v>2</v>
-      </c>
-      <c r="E37" s="10"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="11">
-        <v>0</v>
-      </c>
-      <c r="D38" s="12">
-        <v>1</v>
-      </c>
-      <c r="E38" s="10"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="28"/>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="11">
-        <v>0</v>
-      </c>
-      <c r="D39" s="12">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="28"/>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="11">
-        <v>1</v>
-      </c>
-      <c r="D40" s="12">
-        <v>0</v>
-      </c>
-      <c r="E40" s="10"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="28"/>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="11">
-        <v>0</v>
-      </c>
-      <c r="D41" s="12">
-        <v>1</v>
-      </c>
-      <c r="E41" s="10"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="11">
-        <v>0</v>
-      </c>
-      <c r="D42" s="12">
-        <v>2</v>
-      </c>
-      <c r="E42" s="10"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="28"/>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="11">
-        <v>0</v>
-      </c>
-      <c r="D43" s="12">
-        <v>1</v>
-      </c>
-      <c r="E43" s="10"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="28"/>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="11">
-        <v>1</v>
-      </c>
-      <c r="D44" s="12">
-        <v>0</v>
-      </c>
-      <c r="E44" s="10"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="28"/>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="11">
-        <v>2</v>
-      </c>
-      <c r="D45" s="12">
-        <v>0</v>
-      </c>
-      <c r="E45" s="10"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="28"/>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" s="11">
-        <v>0</v>
-      </c>
-      <c r="D46" s="12">
-        <v>1</v>
-      </c>
-      <c r="E46" s="10"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="28"/>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="11">
-        <v>0</v>
-      </c>
-      <c r="D47" s="12">
-        <v>2</v>
-      </c>
-      <c r="E47" s="10"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="28"/>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="11">
-        <v>0</v>
-      </c>
-      <c r="D48" s="12">
-        <v>2</v>
-      </c>
-      <c r="E48" s="10"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="28"/>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="11">
-        <v>0</v>
-      </c>
-      <c r="D49" s="12">
-        <v>1</v>
-      </c>
-      <c r="E49" s="10"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="28"/>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="11">
-        <v>0</v>
-      </c>
-      <c r="D50" s="12">
-        <v>1</v>
-      </c>
-      <c r="E50" s="10"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="28"/>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="11">
-        <v>0</v>
-      </c>
-      <c r="D51" s="12">
-        <v>1</v>
-      </c>
-      <c r="E51" s="10"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="28"/>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="11">
-        <v>0</v>
-      </c>
-      <c r="D52" s="12">
-        <v>1</v>
-      </c>
-      <c r="E52" s="10"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="28"/>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="11">
-        <v>0</v>
-      </c>
-      <c r="D53" s="12">
-        <v>1</v>
-      </c>
-      <c r="E53" s="10"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="28"/>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="11">
-        <v>0</v>
-      </c>
-      <c r="D54" s="12">
-        <v>1</v>
-      </c>
-      <c r="E54" s="10"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="28"/>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="11">
-        <v>0</v>
-      </c>
-      <c r="D55" s="12">
-        <v>1</v>
-      </c>
-      <c r="E55" s="10"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="28"/>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="13"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="28"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="11">
-        <f>SUM(C7:C55)</f>
-        <v>20</v>
+        <f>SUM(C7:C56)</f>
+        <v>15</v>
       </c>
       <c r="D57" s="11">
-        <f>SUM(D7:D55)</f>
-        <v>46</v>
+        <f>SUM(D7:D56)</f>
+        <v>0</v>
       </c>
       <c r="E57" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add maroon 4 baris
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93EDD47-6038-458A-932D-DE3FD353F86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C348AAD1-29F7-4D5B-B43F-5CB16727D671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Timestamp</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t>Mustrard</t>
+  </si>
+  <si>
+    <t>1. Gamis dewasa Size M</t>
+  </si>
+  <si>
+    <t>2. Kurta Aidil pendek size S X2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Koko Aidil anak Xs </t>
+  </si>
+  <si>
+    <t>4. Khimar nurani size M</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -588,6 +600,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -48161,10 +48179,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E5F31-2BCE-4B36-AB40-B45240226FD3}">
-  <dimension ref="A4:E57"/>
+  <dimension ref="A4:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48263,7 +48281,7 @@
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="36" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="30" t="s">
@@ -48276,7 +48294,7 @@
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="33"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="30" t="s">
         <v>64</v>
       </c>
@@ -48287,7 +48305,7 @@
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="33"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="30" t="s">
         <v>65</v>
       </c>
@@ -48298,7 +48316,7 @@
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="33"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="30" t="s">
         <v>66</v>
       </c>
@@ -48309,7 +48327,7 @@
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="33"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="30" t="s">
         <v>67</v>
       </c>
@@ -48320,7 +48338,7 @@
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="33"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="30" t="s">
         <v>68</v>
       </c>
@@ -48331,7 +48349,7 @@
       <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="33"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="30" t="s">
         <v>69</v>
       </c>
@@ -48342,11 +48360,9 @@
       <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="36" t="s">
-        <v>75</v>
-      </c>
+      <c r="A19" s="37"/>
       <c r="B19" s="30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C19" s="31">
         <v>1</v>
@@ -48355,9 +48371,9 @@
       <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="34"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="30" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C20" s="31">
         <v>2</v>
@@ -48366,9 +48382,9 @@
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="34"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C21" s="31">
         <v>1</v>
@@ -48377,9 +48393,9 @@
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="35"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="30" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C22" s="31">
         <v>1</v>
@@ -48388,26 +48404,48 @@
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="B23" s="29"/>
-      <c r="C23" s="31"/>
+      <c r="A23" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="31">
+        <v>1</v>
+      </c>
       <c r="D23" s="31"/>
       <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="29"/>
-      <c r="C24" s="31"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="31">
+        <v>2</v>
+      </c>
       <c r="D24" s="31"/>
       <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="29"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="31">
+        <v>1</v>
+      </c>
       <c r="D25" s="31"/>
       <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="29"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="31">
+        <v>1</v>
+      </c>
       <c r="D26" s="31"/>
       <c r="E26" s="28"/>
     </row>
@@ -48592,24 +48630,48 @@
       <c r="E56" s="28"/>
     </row>
     <row r="57" spans="2:5">
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="29"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="28"/>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="29"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="28"/>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="29"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="28"/>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" s="29"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="28"/>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="11">
-        <f>SUM(C7:C56)</f>
-        <v>20</v>
+      <c r="C61" s="11">
+        <f>SUM(C7:C60)</f>
+        <v>25</v>
       </c>
-      <c r="D57" s="11">
-        <f>SUM(D7:D56)</f>
+      <c r="D61" s="11">
+        <f>SUM(D7:D60)</f>
         <v>0</v>
       </c>
-      <c r="E57" s="10"/>
+      <c r="E61" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A12:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add 4 green peach
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7C52CA-F4BB-46DE-A87D-388C43F896DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE92ADBA-8FED-47D6-BDFE-60129A0084FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
   <si>
     <t>Timestamp</t>
   </si>
@@ -284,6 +284,21 @@
   </si>
   <si>
     <t>green peach</t>
+  </si>
+  <si>
+    <t>1. koko size : L /lengan : panjang</t>
+  </si>
+  <si>
+    <t>2. gamis dewasa size : XL</t>
+  </si>
+  <si>
+    <t>3. Khimar size: L, Pad:  soft</t>
+  </si>
+  <si>
+    <t>4. gamis anak size : XS no3</t>
+  </si>
+  <si>
+    <t>5. khimar anak size : S</t>
   </si>
 </sst>
 </file>
@@ -48196,8 +48211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E5F31-2BCE-4B36-AB40-B45240226FD3}">
   <dimension ref="A4:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48478,7 +48493,7 @@
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="33"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="29" t="s">
         <v>81</v>
       </c>
@@ -48489,7 +48504,7 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="33"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="29" t="s">
         <v>82</v>
       </c>
@@ -48500,7 +48515,7 @@
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="33"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="29" t="s">
         <v>83</v>
       </c>
@@ -48511,108 +48526,133 @@
       <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="29"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="31">
+        <v>1</v>
+      </c>
       <c r="D31" s="31"/>
       <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="29"/>
-      <c r="C32" s="31"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="31">
+        <v>1</v>
+      </c>
       <c r="D32" s="31"/>
       <c r="E32" s="28"/>
     </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="29"/>
-      <c r="C33" s="31"/>
+    <row r="33" spans="1:5">
+      <c r="A33" s="32"/>
+      <c r="B33" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="31">
+        <v>1</v>
+      </c>
       <c r="D33" s="31"/>
       <c r="E33" s="28"/>
     </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="29"/>
-      <c r="C34" s="31"/>
+    <row r="34" spans="1:5">
+      <c r="A34" s="32"/>
+      <c r="B34" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="31">
+        <v>1</v>
+      </c>
       <c r="D34" s="31"/>
       <c r="E34" s="28"/>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="29"/>
-      <c r="C35" s="31"/>
+    <row r="35" spans="1:5">
+      <c r="A35" s="32"/>
+      <c r="B35" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="31">
+        <v>1</v>
+      </c>
       <c r="D35" s="31"/>
       <c r="E35" s="28"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="1:5">
       <c r="B36" s="29"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="28"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="1:5">
       <c r="B37" s="29"/>
       <c r="C37" s="31"/>
       <c r="D37" s="31"/>
       <c r="E37" s="28"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="1:5">
       <c r="B38" s="29"/>
       <c r="C38" s="31"/>
       <c r="D38" s="31"/>
       <c r="E38" s="28"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="1:5">
       <c r="B39" s="29"/>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
       <c r="E39" s="28"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="1:5">
       <c r="B40" s="29"/>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="1:5">
       <c r="B41" s="29"/>
       <c r="C41" s="31"/>
       <c r="D41" s="31"/>
       <c r="E41" s="28"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="1:5">
       <c r="B42" s="29"/>
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
       <c r="E42" s="28"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="1:5">
       <c r="B43" s="29"/>
       <c r="C43" s="31"/>
       <c r="D43" s="31"/>
       <c r="E43" s="28"/>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="1:5">
       <c r="B44" s="29"/>
       <c r="C44" s="31"/>
       <c r="D44" s="31"/>
       <c r="E44" s="28"/>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="1:5">
       <c r="B45" s="29"/>
       <c r="C45" s="31"/>
       <c r="D45" s="31"/>
       <c r="E45" s="28"/>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="1:5">
       <c r="B46" s="29"/>
       <c r="C46" s="31"/>
       <c r="D46" s="31"/>
       <c r="E46" s="28"/>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="1:5">
       <c r="B47" s="29"/>
       <c r="C47" s="31"/>
       <c r="D47" s="31"/>
       <c r="E47" s="28"/>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="1:5">
       <c r="B48" s="29"/>
       <c r="C48" s="31"/>
       <c r="D48" s="31"/>
@@ -48696,7 +48736,7 @@
       </c>
       <c r="C61" s="11">
         <f>SUM(C7:C60)</f>
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D61" s="11">
         <f>SUM(D7:D60)</f>
@@ -48709,7 +48749,7 @@
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A12:A22"/>
-    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A27:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add 3 frost grey
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE92ADBA-8FED-47D6-BDFE-60129A0084FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C790AD5-A7A6-4589-853B-60C3A29A9A1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
   <si>
     <t>Timestamp</t>
   </si>
@@ -300,6 +300,15 @@
   <si>
     <t>5. khimar anak size : S</t>
   </si>
+  <si>
+    <t xml:space="preserve">1. gamis dewasa size XL 2 pc                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. koko dewasa tgn pendek size XXL   2 pc                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Khimar dewasa 2 pc            </t>
+  </si>
 </sst>
 </file>
 
@@ -530,7 +539,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -618,9 +627,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -48209,10 +48215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E5F31-2BCE-4B36-AB40-B45240226FD3}">
-  <dimension ref="A4:E61"/>
+  <dimension ref="A4:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48267,7 +48273,7 @@
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="33"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="30" t="s">
         <v>59</v>
       </c>
@@ -48278,7 +48284,7 @@
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="33"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="30" t="s">
         <v>60</v>
       </c>
@@ -48289,7 +48295,7 @@
       <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="33"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="30" t="s">
         <v>61</v>
       </c>
@@ -48300,7 +48306,7 @@
       <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="33"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="30" t="s">
         <v>62</v>
       </c>
@@ -48311,44 +48317,44 @@
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="36" t="s">
-        <v>70</v>
-      </c>
+      <c r="A12" s="32"/>
       <c r="B12" s="30" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C12" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="37"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="30" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C13" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="37"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="30" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C14" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="37"/>
+      <c r="A15" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="B15" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" s="31">
         <v>1</v>
@@ -48357,9 +48363,9 @@
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="37"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C16" s="31">
         <v>1</v>
@@ -48368,9 +48374,9 @@
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="37"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="31">
         <v>1</v>
@@ -48379,9 +48385,9 @@
       <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="37"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="31">
         <v>1</v>
@@ -48390,9 +48396,9 @@
       <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="37"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="30" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C19" s="31">
         <v>1</v>
@@ -48401,20 +48407,20 @@
       <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="37"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="30" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C20" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="37"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="30" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C21" s="31">
         <v>1</v>
@@ -48423,9 +48429,9 @@
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="38"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" s="31">
         <v>1</v>
@@ -48434,33 +48440,31 @@
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="36" t="s">
-        <v>75</v>
-      </c>
+      <c r="A23" s="36"/>
       <c r="B23" s="30" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C23" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="34"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="30" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C24" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="34"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="30" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C25" s="31">
         <v>1</v>
@@ -48469,9 +48473,11 @@
       <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="35"/>
+      <c r="A26" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="B26" s="30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C26" s="31">
         <v>1</v>
@@ -48480,22 +48486,20 @@
       <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>80</v>
+      <c r="A27" s="33"/>
+      <c r="B27" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="C27" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="31"/>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="32"/>
-      <c r="B28" s="29" t="s">
-        <v>81</v>
+      <c r="A28" s="33"/>
+      <c r="B28" s="30" t="s">
+        <v>73</v>
       </c>
       <c r="C28" s="31">
         <v>1</v>
@@ -48504,9 +48508,9 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="32"/>
-      <c r="B29" s="29" t="s">
-        <v>82</v>
+      <c r="A29" s="34"/>
+      <c r="B29" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="C29" s="31">
         <v>1</v>
@@ -48515,9 +48519,11 @@
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="32"/>
+      <c r="A30" s="32" t="s">
+        <v>84</v>
+      </c>
       <c r="B30" s="29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C30" s="31">
         <v>1</v>
@@ -48528,7 +48534,7 @@
     <row r="31" spans="1:5">
       <c r="A31" s="32"/>
       <c r="B31" s="29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C31" s="31">
         <v>1</v>
@@ -48539,7 +48545,7 @@
     <row r="32" spans="1:5">
       <c r="A32" s="32"/>
       <c r="B32" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C32" s="31">
         <v>1</v>
@@ -48550,7 +48556,7 @@
     <row r="33" spans="1:5">
       <c r="A33" s="32"/>
       <c r="B33" s="29" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C33" s="31">
         <v>1</v>
@@ -48561,7 +48567,7 @@
     <row r="34" spans="1:5">
       <c r="A34" s="32"/>
       <c r="B34" s="29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" s="31">
         <v>1</v>
@@ -48572,7 +48578,7 @@
     <row r="35" spans="1:5">
       <c r="A35" s="32"/>
       <c r="B35" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" s="31">
         <v>1</v>
@@ -48581,20 +48587,35 @@
       <c r="E35" s="28"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="B36" s="29"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1</v>
+      </c>
       <c r="D36" s="31"/>
       <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="B37" s="29"/>
-      <c r="C37" s="31"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="31">
+        <v>1</v>
+      </c>
       <c r="D37" s="31"/>
       <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="B38" s="29"/>
-      <c r="C38" s="31"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="31">
+        <v>1</v>
+      </c>
       <c r="D38" s="31"/>
       <c r="E38" s="28"/>
     </row>
@@ -48731,25 +48752,43 @@
       <c r="E60" s="28"/>
     </row>
     <row r="61" spans="2:5">
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="29"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="28"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="29"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="28"/>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="29"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="28"/>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="11">
-        <f>SUM(C7:C60)</f>
-        <v>34</v>
+      <c r="C64" s="11">
+        <f>SUM(C7:C63)</f>
+        <v>40</v>
       </c>
-      <c r="D61" s="11">
-        <f>SUM(D7:D60)</f>
+      <c r="D64" s="11">
+        <f>SUM(D7:D63)</f>
         <v>0</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E64" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="A27:A35"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A15:A25"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A7:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
add 3 aqua sea
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4950B7FA-52B7-4E87-AB8E-27EEA4181E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB66EE01-E0C0-4755-AD15-EF6B20E3F3D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
   <si>
     <t>Timestamp</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>aqua sea</t>
+  </si>
+  <si>
+    <t>Dress Aida warna aqua sea size M,1 pcs</t>
+  </si>
+  <si>
+    <t>Koko anak wrna aqua sea size L,1 pcs</t>
+  </si>
+  <si>
+    <t>Koko dewasa wrna aqua sea size M,1 pcs</t>
   </si>
 </sst>
 </file>
@@ -630,12 +639,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -48227,7 +48236,7 @@
   <dimension ref="A4:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A39" sqref="A39:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48269,93 +48278,93 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>1</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="33"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>3</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="33"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>1</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="33"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>2</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="33"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>1</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="33"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>2</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="31"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="33"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>2</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="33"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="31">
         <v>2</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5">
@@ -48365,10 +48374,10 @@
       <c r="B15" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>1</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5">
@@ -48376,10 +48385,10 @@
       <c r="B16" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <v>1</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
@@ -48387,10 +48396,10 @@
       <c r="B17" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <v>1</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5">
@@ -48398,10 +48407,10 @@
       <c r="B18" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <v>1</v>
       </c>
-      <c r="D18" s="32"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5">
@@ -48409,10 +48418,10 @@
       <c r="B19" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>1</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="28"/>
     </row>
     <row r="20" spans="1:5">
@@ -48420,10 +48429,10 @@
       <c r="B20" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>1</v>
       </c>
-      <c r="D20" s="32"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5">
@@ -48431,10 +48440,10 @@
       <c r="B21" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <v>1</v>
       </c>
-      <c r="D21" s="32"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5">
@@ -48442,10 +48451,10 @@
       <c r="B22" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <v>1</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5">
@@ -48453,10 +48462,10 @@
       <c r="B23" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <v>2</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5">
@@ -48464,10 +48473,10 @@
       <c r="B24" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <v>1</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5">
@@ -48475,10 +48484,10 @@
       <c r="B25" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <v>1</v>
       </c>
-      <c r="D25" s="32"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5">
@@ -48488,10 +48497,10 @@
       <c r="B26" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="31">
         <v>1</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5">
@@ -48499,10 +48508,10 @@
       <c r="B27" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <v>2</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="31"/>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5">
@@ -48510,10 +48519,10 @@
       <c r="B28" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="31">
         <v>1</v>
       </c>
-      <c r="D28" s="32"/>
+      <c r="D28" s="31"/>
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5">
@@ -48521,268 +48530,283 @@
       <c r="B29" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="32">
+      <c r="C29" s="31">
         <v>1</v>
       </c>
-      <c r="D29" s="32"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="31">
         <v>1</v>
       </c>
-      <c r="D30" s="32"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="33"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="31">
         <v>1</v>
       </c>
-      <c r="D31" s="32"/>
+      <c r="D31" s="31"/>
       <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="33"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="31">
         <v>1</v>
       </c>
-      <c r="D32" s="32"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="33"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="31">
         <v>1</v>
       </c>
-      <c r="D33" s="32"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="28"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="33"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="31">
         <v>1</v>
       </c>
-      <c r="D34" s="32"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="33"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="31">
         <v>1</v>
       </c>
-      <c r="D35" s="32"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="28"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="33"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="31">
         <v>1</v>
       </c>
-      <c r="D36" s="32"/>
+      <c r="D36" s="31"/>
       <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="33"/>
+      <c r="A37" s="32"/>
       <c r="B37" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="31">
         <v>1</v>
       </c>
-      <c r="D37" s="32"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="33"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="31">
         <v>1</v>
       </c>
-      <c r="D38" s="32"/>
+      <c r="D38" s="31"/>
       <c r="E38" s="28"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="33" t="s">
         <v>94</v>
       </c>
       <c r="B39" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="31">
         <v>1</v>
       </c>
-      <c r="D39" s="32"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="28"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="B40" s="29"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="31">
+        <v>1</v>
+      </c>
+      <c r="D40" s="31"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="B41" s="29"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="31">
+        <v>1</v>
+      </c>
+      <c r="D41" s="31"/>
       <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="B42" s="29"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="31">
+        <v>1</v>
+      </c>
+      <c r="D42" s="31"/>
       <c r="E42" s="28"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="29"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="28"/>
     </row>
     <row r="44" spans="1:5">
       <c r="B44" s="29"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
       <c r="E44" s="28"/>
     </row>
     <row r="45" spans="1:5">
       <c r="B45" s="29"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
       <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:5">
       <c r="B46" s="29"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
       <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:5">
       <c r="B47" s="29"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5">
       <c r="B48" s="29"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
       <c r="E48" s="28"/>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="29"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="28"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="29"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="28"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="29"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
       <c r="E51" s="28"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="29"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
       <c r="E52" s="28"/>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="29"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="28"/>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="29"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
       <c r="E54" s="28"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="29"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
       <c r="E55" s="28"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="29"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
       <c r="E56" s="28"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="29"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
       <c r="E57" s="28"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="29"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
       <c r="E58" s="28"/>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="29"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
       <c r="E59" s="28"/>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="29"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="28"/>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="29"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
       <c r="E61" s="28"/>
     </row>
     <row r="62" spans="2:5">
       <c r="B62" s="29"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
       <c r="E62" s="28"/>
     </row>
     <row r="63" spans="2:5">
       <c r="B63" s="29"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
       <c r="E63" s="28"/>
     </row>
     <row r="64" spans="2:5">
@@ -48791,7 +48815,7 @@
       </c>
       <c r="C64" s="11">
         <f>SUM(C7:C63)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D64" s="11">
         <f>SUM(D7:D63)</f>
@@ -48800,7 +48824,8 @@
       <c r="E64" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A39:A42"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A15:A25"/>
     <mergeCell ref="A30:A38"/>

</xml_diff>

<commit_message>
add 2 frost grey
</commit_message>
<xml_diff>
--- a/order myhijab sarimbit shafeeya.xlsx
+++ b/order myhijab sarimbit shafeeya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\sarimbit-shafeeya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4EF7A4-FF4D-4038-9EBD-EC5E2E9D072C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D182CF3-5C66-4B3D-B223-CDFE4DF091FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
   <si>
     <t>Timestamp</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>5. Koko aidil kids lgn pendek size 3xl</t>
+  </si>
+  <si>
+    <t>1. frost grey/s/aida /gamis</t>
+  </si>
+  <si>
+    <t>2. Frost grey /Koko aidil/ M / tangan panjang bermanset</t>
   </si>
 </sst>
 </file>
@@ -48248,10 +48254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E5F31-2BCE-4B36-AB40-B45240226FD3}">
-  <dimension ref="A4:E69"/>
+  <dimension ref="A4:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48293,7 +48299,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="29" t="s">
@@ -48306,7 +48312,7 @@
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="32"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="30" t="s">
         <v>59</v>
       </c>
@@ -48317,7 +48323,7 @@
       <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="32"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="30" t="s">
         <v>60</v>
       </c>
@@ -48328,7 +48334,7 @@
       <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="32"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="30" t="s">
         <v>61</v>
       </c>
@@ -48339,7 +48345,7 @@
       <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="32"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="30" t="s">
         <v>62</v>
       </c>
@@ -48350,7 +48356,7 @@
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="32"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="30" t="s">
         <v>90</v>
       </c>
@@ -48361,7 +48367,7 @@
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="32"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="30" t="s">
         <v>91</v>
       </c>
@@ -48372,7 +48378,7 @@
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="32"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="30" t="s">
         <v>92</v>
       </c>
@@ -48383,11 +48389,9 @@
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="36" t="s">
-        <v>70</v>
-      </c>
+      <c r="A15" s="37"/>
       <c r="B15" s="30" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="C15" s="31">
         <v>1</v>
@@ -48396,9 +48400,9 @@
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="30" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C16" s="31">
         <v>1</v>
@@ -48407,9 +48411,11 @@
       <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="37"/>
+      <c r="A17" s="36" t="s">
+        <v>70</v>
+      </c>
       <c r="B17" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C17" s="31">
         <v>1</v>
@@ -48420,7 +48426,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="37"/>
       <c r="B18" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="31">
         <v>1</v>
@@ -48431,7 +48437,7 @@
     <row r="19" spans="1:5">
       <c r="A19" s="37"/>
       <c r="B19" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="31">
         <v>1</v>
@@ -48442,7 +48448,7 @@
     <row r="20" spans="1:5">
       <c r="A20" s="37"/>
       <c r="B20" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="31">
         <v>1</v>
@@ -48453,7 +48459,7 @@
     <row r="21" spans="1:5">
       <c r="A21" s="37"/>
       <c r="B21" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="31">
         <v>1</v>
@@ -48464,7 +48470,7 @@
     <row r="22" spans="1:5">
       <c r="A22" s="37"/>
       <c r="B22" s="30" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C22" s="31">
         <v>1</v>
@@ -48475,10 +48481,10 @@
     <row r="23" spans="1:5">
       <c r="A23" s="37"/>
       <c r="B23" s="30" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C23" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="28"/>
@@ -48486,7 +48492,7 @@
     <row r="24" spans="1:5">
       <c r="A24" s="37"/>
       <c r="B24" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="31">
         <v>1</v>
@@ -48497,10 +48503,10 @@
     <row r="25" spans="1:5">
       <c r="A25" s="37"/>
       <c r="B25" s="30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="28"/>
@@ -48508,7 +48514,7 @@
     <row r="26" spans="1:5">
       <c r="A26" s="37"/>
       <c r="B26" s="30" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C26" s="31">
         <v>1</v>
@@ -48519,7 +48525,7 @@
     <row r="27" spans="1:5">
       <c r="A27" s="37"/>
       <c r="B27" s="30" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C27" s="31">
         <v>1</v>
@@ -48530,7 +48536,7 @@
     <row r="28" spans="1:5">
       <c r="A28" s="37"/>
       <c r="B28" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="31">
         <v>1</v>
@@ -48541,7 +48547,7 @@
     <row r="29" spans="1:5">
       <c r="A29" s="37"/>
       <c r="B29" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" s="31">
         <v>1</v>
@@ -48550,9 +48556,9 @@
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="38"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="31">
         <v>1</v>
@@ -48561,11 +48567,9 @@
       <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="36" t="s">
-        <v>75</v>
-      </c>
+      <c r="A31" s="37"/>
       <c r="B31" s="30" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="C31" s="31">
         <v>1</v>
@@ -48574,20 +48578,22 @@
       <c r="E31" s="28"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="34"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="30" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C32" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="31"/>
       <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="34"/>
+      <c r="A33" s="36" t="s">
+        <v>75</v>
+      </c>
       <c r="B33" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" s="31">
         <v>1</v>
@@ -48596,22 +48602,20 @@
       <c r="E33" s="28"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="35"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C34" s="31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" s="31"/>
       <c r="E34" s="28"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>80</v>
+      <c r="A35" s="34"/>
+      <c r="B35" s="30" t="s">
+        <v>73</v>
       </c>
       <c r="C35" s="31">
         <v>1</v>
@@ -48620,9 +48624,9 @@
       <c r="E35" s="28"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="32"/>
-      <c r="B36" s="29" t="s">
-        <v>81</v>
+      <c r="A36" s="35"/>
+      <c r="B36" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="C36" s="31">
         <v>1</v>
@@ -48631,9 +48635,11 @@
       <c r="E36" s="28"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="32"/>
+      <c r="A37" s="32" t="s">
+        <v>84</v>
+      </c>
       <c r="B37" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" s="31">
         <v>1</v>
@@ -48644,7 +48650,7 @@
     <row r="38" spans="1:5">
       <c r="A38" s="32"/>
       <c r="B38" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38" s="31">
         <v>1</v>
@@ -48655,7 +48661,7 @@
     <row r="39" spans="1:5">
       <c r="A39" s="32"/>
       <c r="B39" s="29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C39" s="31">
         <v>1</v>
@@ -48666,7 +48672,7 @@
     <row r="40" spans="1:5">
       <c r="A40" s="32"/>
       <c r="B40" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C40" s="31">
         <v>1</v>
@@ -48677,7 +48683,7 @@
     <row r="41" spans="1:5">
       <c r="A41" s="32"/>
       <c r="B41" s="29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="31">
         <v>1</v>
@@ -48688,7 +48694,7 @@
     <row r="42" spans="1:5">
       <c r="A42" s="32"/>
       <c r="B42" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42" s="31">
         <v>1</v>
@@ -48699,7 +48705,7 @@
     <row r="43" spans="1:5">
       <c r="A43" s="32"/>
       <c r="B43" s="29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" s="31">
         <v>1</v>
@@ -48708,11 +48714,9 @@
       <c r="E43" s="28"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="30" t="s">
-        <v>93</v>
+      <c r="A44" s="32"/>
+      <c r="B44" s="29" t="s">
+        <v>88</v>
       </c>
       <c r="C44" s="31">
         <v>1</v>
@@ -48721,9 +48725,9 @@
       <c r="E44" s="28"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="33"/>
+      <c r="A45" s="32"/>
       <c r="B45" s="29" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C45" s="31">
         <v>1</v>
@@ -48732,9 +48736,11 @@
       <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="33"/>
-      <c r="B46" s="29" t="s">
-        <v>96</v>
+      <c r="A46" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="C46" s="31">
         <v>1</v>
@@ -48745,7 +48751,7 @@
     <row r="47" spans="1:5">
       <c r="A47" s="33"/>
       <c r="B47" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="31">
         <v>1</v>
@@ -48754,102 +48760,112 @@
       <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="B48" s="29"/>
-      <c r="C48" s="31"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="31">
+        <v>1</v>
+      </c>
       <c r="D48" s="31"/>
       <c r="E48" s="28"/>
     </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="29"/>
-      <c r="C49" s="31"/>
+    <row r="49" spans="1:5">
+      <c r="A49" s="33"/>
+      <c r="B49" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="31">
+        <v>1</v>
+      </c>
       <c r="D49" s="31"/>
       <c r="E49" s="28"/>
     </row>
-    <row r="50" spans="2:5">
+    <row r="50" spans="1:5">
       <c r="B50" s="29"/>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
       <c r="E50" s="28"/>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="1:5">
       <c r="B51" s="29"/>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
       <c r="E51" s="28"/>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="1:5">
       <c r="B52" s="29"/>
       <c r="C52" s="31"/>
       <c r="D52" s="31"/>
       <c r="E52" s="28"/>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="1:5">
       <c r="B53" s="29"/>
       <c r="C53" s="31"/>
       <c r="D53" s="31"/>
       <c r="E53" s="28"/>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="1:5">
       <c r="B54" s="29"/>
       <c r="C54" s="31"/>
       <c r="D54" s="31"/>
       <c r="E54" s="28"/>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="1:5">
       <c r="B55" s="29"/>
       <c r="C55" s="31"/>
       <c r="D55" s="31"/>
       <c r="E55" s="28"/>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="1:5">
       <c r="B56" s="29"/>
       <c r="C56" s="31"/>
       <c r="D56" s="31"/>
       <c r="E56" s="28"/>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="1:5">
       <c r="B57" s="29"/>
       <c r="C57" s="31"/>
       <c r="D57" s="31"/>
       <c r="E57" s="28"/>
     </row>
-    <row r="58" spans="2:5">
+    <row r="58" spans="1:5">
       <c r="B58" s="29"/>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
       <c r="E58" s="28"/>
     </row>
-    <row r="59" spans="2:5">
+    <row r="59" spans="1:5">
       <c r="B59" s="29"/>
       <c r="C59" s="31"/>
       <c r="D59" s="31"/>
       <c r="E59" s="28"/>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="1:5">
       <c r="B60" s="29"/>
       <c r="C60" s="31"/>
       <c r="D60" s="31"/>
       <c r="E60" s="28"/>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="1:5">
       <c r="B61" s="29"/>
       <c r="C61" s="31"/>
       <c r="D61" s="31"/>
       <c r="E61" s="28"/>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" spans="1:5">
       <c r="B62" s="29"/>
       <c r="C62" s="31"/>
       <c r="D62" s="31"/>
       <c r="E62" s="28"/>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="1:5">
       <c r="B63" s="29"/>
       <c r="C63" s="31"/>
       <c r="D63" s="31"/>
       <c r="E63" s="28"/>
     </row>
-    <row r="64" spans="2:5">
+    <row r="64" spans="1:5">
       <c r="B64" s="29"/>
       <c r="C64" s="31"/>
       <c r="D64" s="31"/>
@@ -48880,26 +48896,38 @@
       <c r="E68" s="28"/>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="29"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="28"/>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="29"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="28"/>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C69" s="11">
-        <f>SUM(C7:C68)</f>
-        <v>49</v>
+      <c r="C71" s="11">
+        <f>SUM(C7:C70)</f>
+        <v>51</v>
       </c>
-      <c r="D69" s="11">
-        <f>SUM(D7:D68)</f>
+      <c r="D71" s="11">
+        <f>SUM(D7:D70)</f>
         <v>0</v>
       </c>
-      <c r="E69" s="10"/>
+      <c r="E71" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A17:A32"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>